<commit_message>
Final Commit, Project works completely
</commit_message>
<xml_diff>
--- a/Connected Office Test Data.xlsx
+++ b/Connected Office Test Data.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jacqui.Muller\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jandre\Projects\Project-4\CMPG-323-Project-4---31589804\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCAB8EEF-425E-42A8-A7F1-FF25847C778D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Device" sheetId="1" r:id="rId1"/>
@@ -23,7 +22,7 @@
     <definedName name="MOCK_DATA_1" localSheetId="1">Zone!$C$1:$C$201</definedName>
     <definedName name="MOCK_DATA_2" localSheetId="2">Category!$B$1:$C$196</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,8 +32,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="MOCK_DATA" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="MOCK_DATA" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="D:\Downloads\MOCK_DATA.csv" thousands=" " comma="1">
       <textFields count="5">
         <textField/>
@@ -45,7 +44,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="MOCK_DATA(1)" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" name="MOCK_DATA(1)" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="D:\Downloads\MOCK_DATA(1).csv" thousands=" " tab="0" comma="1">
       <textFields count="2">
         <textField/>
@@ -53,7 +52,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="MOCK_DATA(2)" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" name="MOCK_DATA(2)" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="850" sourceFile="D:\Downloads\MOCK_DATA(2).csv" thousands=" " comma="1">
       <textFields count="2">
         <textField/>
@@ -65,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="71">
   <si>
     <t>Status</t>
   </si>
@@ -278,24 +277,12 @@
   </si>
   <si>
     <t>C05</t>
-  </si>
-  <si>
-    <t>Create Test Passed</t>
-  </si>
-  <si>
-    <t>Read Test Passed</t>
-  </si>
-  <si>
-    <t>Update Test Passed</t>
-  </si>
-  <si>
-    <t>Delete Test Passed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -376,15 +363,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="MOCK_DATA" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MOCK_DATA" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="MOCK_DATA(1)" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MOCK_DATA(1)" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="MOCK_DATA(2)" connectionId="3" xr16:uid="{00000000-0016-0000-0200-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="MOCK_DATA(2)" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -683,7 +670,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -907,7 +894,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1037,7 +1024,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1124,11 +1111,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{243FE4D3-E987-44A9-BA20-E766DD09E091}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1141,393 +1128,393 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>74</v>
+        <v>57</v>
+      </c>
+      <c r="B1" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E8" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E17" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E18" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E20" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E22" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E23" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1535,16 +1522,16 @@
         <v>56</v>
       </c>
       <c r="B24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E24" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>